<commit_message>
Update with full data through end of Ravinia 2024
</commit_message>
<xml_diff>
--- a/input/ravinia_data_2024.xlsx
+++ b/input/ravinia_data_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcong\Dropbox\github\ravinia2024\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B8273C-3D40-41E0-B1D0-1C3CF85FC32F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE0A5AF-28D1-45F1-9B86-FF32CCC4F83A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A9F4FDC-F987-4771-878E-F4362E2E24DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="205">
   <si>
     <t>band</t>
   </si>
@@ -430,6 +430,225 @@
   </si>
   <si>
     <t>The Grammy-winning baroque orchestra Apollo's Fire, called "a gem of an ensemble" by the New York Times, returns to Ravinia with artistic director, conductor, and harpsichordist Jeannette Sorrell for their artfully curated program Vivaldi's Four Seasons Rediscovered. The group presents Vivaldi's revolutionary acts of musical storytelling as they were meant to be performed, bringing his pictorial descriptions to life. From bird calls and storms to a barking dog, flies and wasps, drunken peasants, an exhilarating fox hunt, and more, audiences around the world have been enchanted by this touring production.</t>
+  </si>
+  <si>
+    <t>CSO &amp; Jonathan Rush</t>
+  </si>
+  <si>
+    <t>Conductor Jonathan Rush, a protégé of Marin Alsop and last summer's Lead Seminario Conductor, joins the Chicago Symphony Orchestra for Hector Berlioz's Symphonie fantastique and more. A graduate of Peabody Conservatory, Rush grew up steeped in gospel and other roots-based genres. "What I bring is something so different," he said. "My foundation was gospel. I'm not just going to bring classical, I'm going to bring soul ... the whole music world that makes up Jonathan Rush. People my age, we have something to offer, and it’s completely different.”</t>
+  </si>
+  <si>
+    <t>Rachel Barton Pine</t>
+  </si>
+  <si>
+    <t>Chicago native and recurrent CSO collaborator Rachel Barton Pine takes the stage with Rush and the orchestra for the CSO premiere of José White Lafitte's Violin Concerto in F-sharp Minor plus Niccolò Paganini's La Campanella. The Washington Post described her as "an exciting, boundary-defying performer." Pine "displays a power and confidence that puts her in the top echelon."</t>
+  </si>
+  <si>
+    <t>Matthew Polenzani &amp; Kevin Murphy</t>
+  </si>
+  <si>
+    <t>American tenor Matthew Polenzani, who boasts a "wonderfully fresh and robust voice, with clarion top notes and a gift for sweet phrasing," (San Francisco Chronicle), returns to Ravinia with pianist Kevin Murphy. Polenzani's 2023/24 season includes starring as the title character in Mozart’s La clemenza di Tito at the Wiener Staatsoper, a role debut as Orombello in Bellini’s rarely performed Beatrice di Tenda at Teatro di San Carlo, a return to the Metropolitan Opera as Rodolfo in La Bohème, and another role debut as Florestan in Fidelio at Staatsoper Hamburg. He frequently performs with premier ensembles in the United States and Europe, including the Berlin Philharmonic, Boston Symphony Orchestra, Chicago Symphony Orchestra, Cleveland Orchestra, Los Angeles Philharmonic, New York Philharmonic.</t>
+  </si>
+  <si>
+    <t>Gaelic Storm</t>
+  </si>
+  <si>
+    <t>The High Kings</t>
+  </si>
+  <si>
+    <t>Gaelic Storm and The High Kings are back on tour together as both groups make their Ravinia debuts. Gaelic Storm was formed in California and has toured and recorded for over 20 years, attributing their great success to a notably dedicated fan base. They combine traditional folk music from Ireland and Scotland with Celtic rock. Tunes like "Blarney Pilgrim," "John Ryan's Polka," "Kesh Jig," and "Drowsy Maggie" charmed audiences around the world as the group appeared as the steerage band in the blockbuster film Titanic.</t>
+  </si>
+  <si>
+    <t>The High Kings, founded in Dublin in 2007, is an Irish folk group with five studio albums and four live recordings to their name. They have performed extensively in their native Ireland and across Europe and the USA. Following a performance in front of President Barack Obama, they were invited to feature at the White House's 2012 St. Patrick's Day celebration.</t>
+  </si>
+  <si>
+    <t>O.A.R</t>
+  </si>
+  <si>
+    <t>Fitz and the Tantrums</t>
+  </si>
+  <si>
+    <t>For over 25 years, O.A.R. have embodied the kind of joyfully communal spirit that’s transcendent for both artist and audience alike. Since forming in Maryland in 1996, the multi-platinum-selling band have merged their musical DNA into a free-flowing sound and exhilarating live show, repeatedly selling out legendary venues like Madison Square Garden thanks to their massively devoted community of fans. In a thrilling new chapter for the ever-evolving collective, O.A.R.’s tenth studio album The Arcade marks their most collaborative effort yet: a boldly unpredictable body of work that fully showcases the extraordinary expanse of their singular musicality.</t>
+  </si>
+  <si>
+    <t>Special guest Fitz &amp; the Tantrums, a soul influenced indie-pop band hailing from Los Angeles, shares the stage. "Fitz &amp; the Tantrums is the kind of band that communicates best in concert," says the Los Angeles Times, "but [the album Pickin' Up The Pieces] serves as a fine proxy and party-starter."</t>
+  </si>
+  <si>
+    <t>indie</t>
+  </si>
+  <si>
+    <t>The Roots</t>
+  </si>
+  <si>
+    <t>Hailing from Philadelphia and founded by Tariq "Black Thought" Trotter and Ahmir "Questlove" Thompson, The Roots approach hip hop with live instruments and touches of jazz and improvisatory pop. They won their first Grammy with "You Got Me," featuring Erykah Badu, and went on to win more with "Hang On in There" and the album Wake Up!, both in collaboration with John Legend. They have played as the house band on both of Jimmy Fallon's late night shows, serving that role since 2009.</t>
+  </si>
+  <si>
+    <t>Digable Planets</t>
+  </si>
+  <si>
+    <t>Digable Planets burst into the music scene in the early '90s with their Grammy Award-winning "Rebirth Of Slick (Cool Like Dat)." Made up of Ishmael "Butterfly" Butler, Craig "Doodlebug" Irving, and Mary Ann “Ladybug Mecca” Vieira, the trio carved out a unique style of jazz-informed hip hop. Digable Planets' debut album, Reachin’ (A New Refutation of Time And Space), was certified gold and praised by Pitchfork as “a world within a world, complete with its own language and monuments.” Melding jazz samples and complex rhymes, they have touched on themes from the nuances of city life to women's rights.</t>
+  </si>
+  <si>
+    <t>Arrested Development</t>
+  </si>
+  <si>
+    <t>Hip-hop trailbalzer Arrested Development has been a champion of cultural consciousness and empowerment since their foundation in the early 90's. Their merge of African sounds, rhythm, and fashion has left a notable mark on hip hop culture, and they continue a mission of social activism through support of groups like the National Coalition of The Homeless and the African National Congress. The album 3 Years, 5 Months and 2 Days in the Life of... earned Arrested Development two Grammy Awards, two MTV awards, a Soul Train Music Award, and the NAACP Image Award.</t>
+  </si>
+  <si>
+    <t>Samara Joy</t>
+  </si>
+  <si>
+    <t>24-year-old jazz phenom Samara Joy makes her Ravinia debut following the release of her first album on Verve Records, Linger Awhile. That record reached number one on the Billboard Jazz Albums chart, after Joy won the Sarah Vaughan International Jazz Vocal Competition and was named Best New Artist by JazzTimes. "Listening to Joy's approach is a revelation," says All About Jazz. "The ease with which her voice moves, her ability to sing with and without vibrato ... Her phrasing is always spot-on." Joy's distinct vocal stylings have already earned her fans like Anita Baker and Regina King.</t>
+  </si>
+  <si>
+    <t>Stella Chen, Matthew Lipman, Brannon Cho Trio</t>
+  </si>
+  <si>
+    <t>Violinist Stella Chen and violist Matthew Lipman, both alumni of the Ravinia Steans Music Institute, join cellist Brannon Cho for an afternoon of chamber music trios. At Bennett Gordon Hall, they interpret Ludwig van Beethoven's String Trio No. 3 in G major, Gideon Klein's String Trio, and Wolfgang Amadeus Mozart's Divertimento in E-flat major.</t>
+  </si>
+  <si>
+    <t>Third Coast Percussion &amp; Sergio Clarice Assad</t>
+  </si>
+  <si>
+    <t>The Grammy-nominated project Archetypes, a production by Third Coast Percussion and Sergio and Clarice Assad, comes to Ravinia's Martin Theatre. This collaboratively composed work features twelve musical portraits of timeless character types that appear in stories, legends, and myths throughout the world, from The Rebel and The Explorer to The Orphan and The Caregiver. The Classical Music Sentinel calls the work "an abundance of ear candy."</t>
+  </si>
+  <si>
+    <t>Zlatomir Fung &amp; Dina Vainshtein</t>
+  </si>
+  <si>
+    <t>Ravinia Steans Music Institute alumn Zlatomir Fung is the youngest cellist ever to win First Prize at the International Tchaikovsky Competition, currently serving as the Royal Philharmonic Orchestra's Artist-in-Residence and featuring recently with the Cleveland Orchestra, Baltimore Symphony, and London Philharmonic Orchestra. He shares the stage with pianist Dina Vainshtein for an evening of chamber music at Bennett Gordon Hall.</t>
+  </si>
+  <si>
+    <t>ZZ Top</t>
+  </si>
+  <si>
+    <t>Lynyrd Skynyrd</t>
+  </si>
+  <si>
+    <t>Two titans of American classic rock, ZZ Top and Lynyrd Skynyrd, return to Ravinia on their co-headlining The Sharp Dressed Simple Man Tour. ZZ Top has been at it for well over a half century delivering rock, blues, and boogie on stage and in the studio. With iconography as distinctive as their sound, the band is globally recognized for their beards, hotrod cars, and spinning guitars, all of which transcend geography and language. They have sold hundreds of millions of records over the course of their career, have been officially designated as Heroes of The State of Texas, inducted into the Rock and Roll Hall of Fame, and have been referenced in countless cartoons and sitcoms.</t>
+  </si>
+  <si>
+    <t>As Lynyrd Skynyrd celebrates the 50th anniversary of the band’s critically acclaimed debut album, they resonate as deeply with their multi-generational fan base today as when they first emerged out of Jacksonville, Florida in 1973. With a catalog of over 60 albums, billions of streams, and tens of millions of records sold, Rock and Roll Hall of Famers Lynyrd Skynyrd remain a cultural icon that appeal to all generations. The rock and roll powerhouse continually tours, and as Ronnie Van Zant shares, “it’s about the legacy of Lynyrd Skynyrd, and what it stands for, what the fans are all about. There’s nothing like getting out there playing a great show with Skynyrd and seeing people love this music.”</t>
+  </si>
+  <si>
+    <t>Fyütch</t>
+  </si>
+  <si>
+    <t>Fyütch is a Grammy-nominated music and social justice artist, educator, and content creator of choice for live events, corporate workshops, K-12 classrooms, assemblies, and residencies. He uses hip hop, spoken word, and visual storytelling to create unique all-ages experiences that promote racial equity and liberation.</t>
+  </si>
+  <si>
+    <t>TLC</t>
+  </si>
+  <si>
+    <t>R&amp;B supergroup TLC and Jamaican dancehall icon Shaggy join forces for a night of their decades of multi-Grammy-winning hits, from T-Boz and Chilli’s chart-toppers “No Scrubs,” “Unpretty,” “Creep,” and “Waterfalls” to the reggae fusion artist’s “It Wasn’t Me,” “Boombastic,” and “Angel.” With over 85 million records on their ledger worldwide, TLC is the best-selling American ‘girl group’ of all time and highlighted by Billboard as the seventh most successful artist of the 1990s. They became the first female group to earn a Diamond Award in record sales with 1994’s CrazySexyCool.</t>
+  </si>
+  <si>
+    <t>reggae</t>
+  </si>
+  <si>
+    <t>Similarly, Shaggy is the only Diamond-selling dancehall artist in music history with more than 40 million albums moved. Including 2000’s number-one Hot Shot, four of his albums have been top-40 hits, and he ranks among the top three streamed reggae artists on Spotify.</t>
+  </si>
+  <si>
+    <t>Shaggy</t>
+  </si>
+  <si>
+    <t>David Kaplan</t>
+  </si>
+  <si>
+    <t>Pianist David Kaplan, an alumn of the Ravinia Steans Music Institute, returns to Bennett Gordon Hall for Quasi una fantastia. Kaplan gives the Ravinia premieres of György Ligeti's Musica ricercata No. 1, Christopher Cerrone's Passagework, Louis Couperin's Unmeasured Prelude No. 13 in F major, Anthony Cheung's Holding Patterns, Kaija Saariaho's Ballade, and Andrea Casarrubios' Sandglass alongside works by Johannes Brahms, Ludwig van Beethoven, and more.</t>
+  </si>
+  <si>
+    <t>Yevgeny Kutik &amp; Renana Gutman</t>
+  </si>
+  <si>
+    <t>Violinist Yevgeny Kutik and pianist Renana Gutman, the latter a Ravinia Steans Music Institute alumna, perform selections from their Music from the Suitcase project with surprise repertoire announced from the stage. They are in the spotlight at Bennett Gordon Hall for three performances featuring music by Felix Mendelssohn, Sergei Prokofiev, Peter Ilyich Tchaikovsky, Darius Milhaud, and many more.</t>
+  </si>
+  <si>
+    <t>Big Drum / Small World</t>
+  </si>
+  <si>
+    <t>Jason Isbell and the 400 Unit</t>
+  </si>
+  <si>
+    <t>Jason Isbell and the 400 Unit and Alejandro Escovedo both return to Ravinia. Isbell formed the 400 Unit with musicians mainly hailing from the area around Muscle Shoals, Alabama, releasing their first album together in 2009. Their second studio album, Here We Rest, featured the Americana Music Awards Song of the Year "Alabama Pines." The group went on to win the Grammy Award for Best Americana Album, and Isbell won the Grammy Award for Best American Roots Song in 2017. Their appearance at Ravinia follows another big year at the Grammys, where Isbell won the Best American Roots Song for "Cast Iron Skillet" and the band was awarded Best Americana Album for 2023's Weathervanes.</t>
+  </si>
+  <si>
+    <t>Alejandro Escovedo</t>
+  </si>
+  <si>
+    <t>Alejandro Escovedo has had “one of the most fascinating paths in music," (NPR Music) and on his latest album explores his a one-of-a-kind musical life from the 1970's New York punk scene to his time as Austin's hometown hero. Echo Dancing traces his identity as “a literate soul and true punk" (The New Yorker).</t>
+  </si>
+  <si>
+    <t>punk</t>
+  </si>
+  <si>
+    <t>Dame Jane Glover &amp; Anthony McGill</t>
+  </si>
+  <si>
+    <t>Music by Johann Sebastian Bach, Wolfgang Amadeus Mozart, and George Frideric Handel rings out at the Martin Theatre as Music of the Baroque, led by Dame Jane Glover, and Anthony McGill all return to Ravinia. “Lyric Opera of Chicago and the Chicago Symphony Orchestra may be the big guys on the local classical music scene, but in terms of sheer quality of performance … Music of the Baroque inhabits the same stratosphere," says the Chicago Sun-Times of this leading ensemble. Also in the limelight is Anthony McGill, a clarinetist whose playing is known for its “trademark brilliance, penetrating sound, and rich character” (New York TImes).</t>
+  </si>
+  <si>
+    <t>Crowded House</t>
+  </si>
+  <si>
+    <t>Founded in Australia in 1985, powerhouse rock group Crowded House's catalogue of hits includes "Don't Dream It's Over," "Weather With You," "Better Be Home Soon," and "Fall At Your Feet." Vocalist, guitarist, and songwriter Neil Finn has led the band through multiple line-ups and artistic iterations, and "has consistently proven his knack for crafting high-quality songs that combine irresistible melodies with meticulous lyrical detail." (Allmusic) The band appears for the first time ever at Ravinia just out of the studio with their new single, "Oh Hi."</t>
+  </si>
+  <si>
+    <t>Aznavoorian Duo</t>
+  </si>
+  <si>
+    <t>Ravinia Steans Music Institute alum Ani Aznavoorian, a cellist whose “scorchingly committed performances … wring every last drop of emotion out of the music," (The Strad) and Lincoln Trio's Marta Aznavoorian, "a pianist of exceptionally finished technique and purity of musical impulse" (The Boston Globe) return to Ravinia to perform selections from their 2022 debut album, Gems from Armenia. This mesmerizing concert will explore legacies from Armenia to America, with works by Peter Boyer, Leo Sowerby, Komitas Vardapet, Samuel Barber, and more.</t>
+  </si>
+  <si>
+    <t>Joffrey Ballet</t>
+  </si>
+  <si>
+    <t>Chicago's own Joffrey Ballet is back in Ravinia's Pavilion for an evening of dance. One of the leading American companies, Joffrey Ballet seeks to advance dance through artistic excellence, innovation, and arts education. In new choreography by Houston Thomas, the company celebrates the music and life of jazz legend Ramsey Lewis, and works by Cathy Marston and Nicolas Blanc will be featured with live musicians.</t>
+  </si>
+  <si>
+    <t>Michael Serafini</t>
+  </si>
+  <si>
+    <t>Garrett David</t>
+  </si>
+  <si>
+    <t>Lucy Stoole</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Through the mentorship of Chez Damier, studying behind the desk at Gramaphone Records, and being at the helm of smartbar’s wildly successful Queen! party, Garrett David has spent the past decade developing his unmistakable style and ability to hypnotize the dance floor. His meticulous approach and underground attitude shines through his production, releasing lush and skittery tunes on prestigious labels such as Courtesy of Balance, Smallville, Residual, and his own imprint, Global Swing.</t>
+  </si>
+  <si>
+    <t>Michael Serafini first got his start in Chicago nightlife in the ’80s working for Berlin nightclub as a video jockey and remixer. Under the mentorship of close friends Terri Bristol and Ralphi Rosario, Serafini began DJing regularly in the early ’90s and took up a position at one of Chicago house’s most famous institutions, Gramaphone Records. As his experience grew, so did his reputation, later landing a residency at Boom Boom Room, then the city’s longest-running house night. In 2007, Serafini took over ownership of Gramaphone Records, which he still operates today.</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>drag</t>
+  </si>
+  <si>
+    <t>Nico is the anti-socialite party girl that brings shots and chaotic energy to the room, straight from the runway to the punk show. She’s rough around the edges with a face that’s always blended for the HD.</t>
+  </si>
+  <si>
+    <t>Lucy Stoole, Chicago’s Black Bearded Beauty, is a Windy City-based drag performer, artist, and activist with an international presence. She’s an Out 100 honoree, two-time Drag Queen of the Year, and entrepreneur.</t>
+  </si>
+  <si>
+    <t>As part of Ravinia's Kids Concert Series, the Joffrey Ballet delights audiences of all ages onstage at the Pavilion. They present Rita Finds Home, a collaboration with the Miami City Ballet and a women-led creative team. The production centers on Rita, a young artist who paints and dreams of one day living in the big city despite the lush tropical island in which she now lives. Rita must go on a journey that helps her redefine "home."</t>
+  </si>
+  <si>
+    <t>Julieta Venegas</t>
+  </si>
+  <si>
+    <t>Mexican-American singer-songwriter Julieta Venegas plays 17 instruments – including guitar, accordion, and keyboard – and is known for her deeply personal takes on Mexican rock, indie, and pop music. She has won eight Latin Grammy Awards, seven MTV Awards, and two Billboard Music Awards. Hits like "Me Voy" and "Sería Feliz" are audience favorites in the Americas and around the world.</t>
+  </si>
+  <si>
+    <t>La Santa Cecilia</t>
+  </si>
+  <si>
+    <t>La Santa Cecilia is a band that exemplifies a modern-day hybrid of Latin culture, rock, and world music. The group draws inspiration from all over the world, utilizing Pan-American rhythms including cumbia, bossa-nova, rumba, bolero, tango, jazz and klezmer music. Their first studio album, Treinta Días, won a Grammy for Best Latin Rock, Urban or Alternative Album.</t>
   </si>
 </sst>
 </file>
@@ -783,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A578CDB-7E3F-482F-9D54-63FDEC0EBE06}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,83 +1964,545 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>113</v>
+      </c>
       <c r="B84" s="1">
         <v>45520</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>113</v>
+      </c>
       <c r="B85" s="1">
         <v>45521</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>132</v>
+      </c>
       <c r="B86" s="1">
         <v>45522</v>
       </c>
+      <c r="C86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D86" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>134</v>
+      </c>
       <c r="B87" s="1">
-        <v>45523</v>
+        <v>45522</v>
+      </c>
+      <c r="C87" t="s">
+        <v>135</v>
+      </c>
+      <c r="D87" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B88" s="1">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>136</v>
+      </c>
+      <c r="B89" s="1">
         <v>45524</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="1">
-        <v>45525</v>
+      <c r="C89" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B90" s="1">
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" s="1">
         <v>45526</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="1">
+      <c r="C91" t="s">
+        <v>140</v>
+      </c>
+      <c r="D91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="1">
+        <v>45526</v>
+      </c>
+      <c r="C92" t="s">
+        <v>141</v>
+      </c>
+      <c r="D92" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="1">
         <v>45527</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="1">
+      <c r="C93" t="s">
+        <v>144</v>
+      </c>
+      <c r="D93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>143</v>
+      </c>
+      <c r="B94" s="1">
+        <v>45527</v>
+      </c>
+      <c r="C94" t="s">
+        <v>145</v>
+      </c>
+      <c r="D94" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>147</v>
+      </c>
+      <c r="B95" s="1">
         <v>45528</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B93" s="1">
+      <c r="C95" t="s">
+        <v>148</v>
+      </c>
+      <c r="D95" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>149</v>
+      </c>
+      <c r="B96" s="1">
+        <v>45528</v>
+      </c>
+      <c r="C96" t="s">
+        <v>150</v>
+      </c>
+      <c r="D96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>151</v>
+      </c>
+      <c r="B97" s="1">
+        <v>45528</v>
+      </c>
+      <c r="C97" t="s">
+        <v>152</v>
+      </c>
+      <c r="D97" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>153</v>
+      </c>
+      <c r="B98" s="1">
         <v>45529</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="1">
+      <c r="C98" t="s">
+        <v>154</v>
+      </c>
+      <c r="D98" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>155</v>
+      </c>
+      <c r="B99" s="1">
+        <v>45529</v>
+      </c>
+      <c r="C99" t="s">
+        <v>156</v>
+      </c>
+      <c r="D99" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B100" s="1">
         <v>45530</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B95" s="1">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>157</v>
+      </c>
+      <c r="B101" s="1">
         <v>45531</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B96" s="1">
+      <c r="C101" t="s">
+        <v>158</v>
+      </c>
+      <c r="D101" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>159</v>
+      </c>
+      <c r="B102" s="1">
         <v>45532</v>
       </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B97" s="1">
+      <c r="C102" t="s">
+        <v>160</v>
+      </c>
+      <c r="D102" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>161</v>
+      </c>
+      <c r="B103" s="1">
         <v>45533</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B98" s="1">
+      <c r="C103" t="s">
+        <v>163</v>
+      </c>
+      <c r="D103" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>162</v>
+      </c>
+      <c r="B104" s="1">
+        <v>45533</v>
+      </c>
+      <c r="C104" t="s">
+        <v>164</v>
+      </c>
+      <c r="D104" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B105" s="1">
         <v>45534</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B99" s="1">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>165</v>
+      </c>
+      <c r="B106" s="1">
         <v>45535</v>
+      </c>
+      <c r="C106" t="s">
+        <v>166</v>
+      </c>
+      <c r="D106" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>167</v>
+      </c>
+      <c r="B107" s="1">
+        <v>45535</v>
+      </c>
+      <c r="C107" t="s">
+        <v>168</v>
+      </c>
+      <c r="D107" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="1">
+        <v>45535</v>
+      </c>
+      <c r="C108" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" s="1">
+        <v>45536</v>
+      </c>
+      <c r="C109" t="s">
+        <v>173</v>
+      </c>
+      <c r="D109" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B110" s="1">
+        <v>45537</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B111" s="1">
+        <v>45538</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B112" s="1">
+        <v>45539</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>174</v>
+      </c>
+      <c r="B113" s="1">
+        <v>45540</v>
+      </c>
+      <c r="C113" t="s">
+        <v>175</v>
+      </c>
+      <c r="D113" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B114" s="1">
+        <v>45541</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>176</v>
+      </c>
+      <c r="B115" s="1">
+        <v>45542</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>177</v>
+      </c>
+      <c r="B116" s="1">
+        <v>45543</v>
+      </c>
+      <c r="C116" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>179</v>
+      </c>
+      <c r="B117" s="1">
+        <v>45543</v>
+      </c>
+      <c r="C117" t="s">
+        <v>180</v>
+      </c>
+      <c r="D117" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B118" s="1">
+        <v>45544</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>182</v>
+      </c>
+      <c r="B119" s="1">
+        <v>45545</v>
+      </c>
+      <c r="C119" t="s">
+        <v>183</v>
+      </c>
+      <c r="D119" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>184</v>
+      </c>
+      <c r="B120" s="1">
+        <v>45546</v>
+      </c>
+      <c r="C120" t="s">
+        <v>185</v>
+      </c>
+      <c r="D120" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>186</v>
+      </c>
+      <c r="B121" s="1">
+        <v>45547</v>
+      </c>
+      <c r="C121" t="s">
+        <v>187</v>
+      </c>
+      <c r="D121" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>188</v>
+      </c>
+      <c r="B122" s="1">
+        <v>45548</v>
+      </c>
+      <c r="C122" t="s">
+        <v>189</v>
+      </c>
+      <c r="D122" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>190</v>
+      </c>
+      <c r="B123" s="1">
+        <v>45549</v>
+      </c>
+      <c r="C123" t="s">
+        <v>195</v>
+      </c>
+      <c r="D123" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>191</v>
+      </c>
+      <c r="B124" s="1">
+        <v>45549</v>
+      </c>
+      <c r="C124" t="s">
+        <v>194</v>
+      </c>
+      <c r="D124" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>192</v>
+      </c>
+      <c r="B125" s="1">
+        <v>45549</v>
+      </c>
+      <c r="C125" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>193</v>
+      </c>
+      <c r="B126" s="1">
+        <v>45549</v>
+      </c>
+      <c r="C126" t="s">
+        <v>198</v>
+      </c>
+      <c r="D126" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>188</v>
+      </c>
+      <c r="B127" s="1">
+        <v>45549</v>
+      </c>
+      <c r="C127" t="s">
+        <v>200</v>
+      </c>
+      <c r="D127" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>201</v>
+      </c>
+      <c r="B128" s="1">
+        <v>45550</v>
+      </c>
+      <c r="C128" t="s">
+        <v>202</v>
+      </c>
+      <c r="D128" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>203</v>
+      </c>
+      <c r="B129" s="1">
+        <v>45550</v>
+      </c>
+      <c r="C129" t="s">
+        <v>204</v>
+      </c>
+      <c r="D129" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>